<commit_message>
Email support added, fixed Report class issues
Added pom dependency.
Added sendEmail method to the controller.
Added the last details to the AirportView (send email function)
</commit_message>
<xml_diff>
--- a/target/classes/fullDataz.xlsx
+++ b/target/classes/fullDataz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chibi\IdeaProjects\ExcelPractice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chibi\IdeaProjects\solidPrj\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB5D9E0-7C35-41DD-8583-6DD989ACDDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7028F373-B35E-4E71-94B4-E04EF60CB42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="210" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Origin</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
     <t>Departure Time</t>
   </si>
   <si>
@@ -83,6 +77,51 @@
   </si>
   <si>
     <t>California</t>
+  </si>
+  <si>
+    <t>Aircraft Capacity</t>
+  </si>
+  <si>
+    <t>Aircraft Range</t>
+  </si>
+  <si>
+    <t>Origin Country</t>
+  </si>
+  <si>
+    <t>Origin City</t>
+  </si>
+  <si>
+    <t>Destination City</t>
+  </si>
+  <si>
+    <t>Destination Country</t>
+  </si>
+  <si>
+    <t>Departure Date</t>
+  </si>
+  <si>
+    <t>Arrival Date</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Tegucigalpa</t>
+  </si>
+  <si>
+    <t>Guadalajara</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>A, B, C</t>
+  </si>
+  <si>
+    <t>Not-Avianca</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -118,8 +157,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,15 +475,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,92 +506,209 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="2">
+        <v>44319</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="M2" s="2">
+        <v>44320</v>
+      </c>
+      <c r="N2" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2">
+        <v>44348</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="M3" s="2">
+        <v>44348</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="O3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="P3" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
-        <v>2021</v>
-      </c>
-      <c r="H2">
-        <v>130</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>2021</v>
-      </c>
-      <c r="H3">
-        <v>130</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2">
+        <v>44348</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="M4" s="2">
+        <v>44348</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>